<commit_message>
Skip Mr.Tùng class :(
</commit_message>
<xml_diff>
--- a/DB_CollegeManage/hello.xlsx
+++ b/DB_CollegeManage/hello.xlsx
@@ -12,7 +12,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+  <si>
+    <t>Davce</t>
+  </si>
+  <si>
+    <t>90K</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>Rupert</t>
+  </si>
+  <si>
+    <t>Daeve</t>
+  </si>
+  <si>
+    <t>Dxeave</t>
+  </si>
+  <si>
+    <t>Darfve</t>
+  </si>
+  <si>
+    <t>Daeedve</t>
+  </si>
+  <si>
+    <t>Davxfe</t>
+  </si>
+  <si>
+    <t>Dasve</t>
+  </si>
   <si>
     <t>Sonya</t>
   </si>
@@ -20,10 +50,7 @@
     <t>75K</t>
   </si>
   <si>
-    <t>SALES</t>
-  </si>
-  <si>
-    <t>Rupert</t>
+    <t>Davqe</t>
   </si>
   <si>
     <t>Kris</t>
@@ -33,9 +60,6 @@
   </si>
   <si>
     <t>Dave</t>
-  </si>
-  <si>
-    <t>90K</t>
   </si>
 </sst>
 </file>
@@ -80,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,7 +112,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>7.0</v>
+        <v>99.0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -105,13 +129,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8.0</v>
+        <v>89.0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -122,18 +146,171 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>779.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>9.0</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>